<commit_message>
up to date data
</commit_message>
<xml_diff>
--- a/streamlit/Houses_Cleaned.xlsx
+++ b/streamlit/Houses_Cleaned.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F703"/>
+  <dimension ref="A1:F702"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14714,14 +14714,14 @@
         <v>220000</v>
       </c>
       <c r="B600" t="n">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C600" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D600" t="inlineStr">
         <is>
-          <t>Debrecen, Bethlen</t>
+          <t>Debrecen, Nyár street</t>
         </is>
       </c>
       <c r="E600" t="n">
@@ -14729,7 +14729,7 @@
       </c>
       <c r="F600" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/luxury-apartment-for-rent-in-the-city-center/</t>
+          <t>https://www.findahome.hu/ingatlanok/nyar-street-2-bedroom-living-room-flat-for-rent/</t>
         </is>
       </c>
     </row>
@@ -14810,14 +14810,14 @@
         <v>220000</v>
       </c>
       <c r="B604" t="n">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C604" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D604" t="inlineStr">
         <is>
-          <t>Debrecen, Nyár street</t>
+          <t>Debrecen, Bethlen</t>
         </is>
       </c>
       <c r="E604" t="n">
@@ -14825,7 +14825,7 @@
       </c>
       <c r="F604" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/nyar-street-2-bedroom-living-room-flat-for-rent/</t>
+          <t>https://www.findahome.hu/ingatlanok/luxury-apartment-for-rent-in-the-city-center/</t>
         </is>
       </c>
     </row>
@@ -14882,14 +14882,14 @@
         <v>220000</v>
       </c>
       <c r="B607" t="n">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C607" t="n">
         <v>3</v>
       </c>
       <c r="D607" t="inlineStr">
         <is>
-          <t>Debrecen, Serház</t>
+          <t>Debrecen, Hatvan Corner</t>
         </is>
       </c>
       <c r="E607" t="n">
@@ -14897,7 +14897,7 @@
       </c>
       <c r="F607" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/debrecen-serhaz-utca-2-bedroom-living-room-flat-for-rent/</t>
+          <t>https://www.findahome.hu/ingatlanok/hatvan-corner-2-bedroom-living-room-flat-for-rent/</t>
         </is>
       </c>
     </row>
@@ -14930,14 +14930,14 @@
         <v>220000</v>
       </c>
       <c r="B609" t="n">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="C609" t="n">
         <v>3</v>
       </c>
       <c r="D609" t="inlineStr">
         <is>
-          <t>Debrecen, Hatvan Corner</t>
+          <t>Debrecen, Arany János</t>
         </is>
       </c>
       <c r="E609" t="n">
@@ -14945,7 +14945,7 @@
       </c>
       <c r="F609" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/hatvan-corner-2-bedroom-living-room-flat-for-rent/</t>
+          <t>https://www.findahome.hu/ingatlanok/city-center-2-bedroom-american-style-kitchen-apartment-for-rent/</t>
         </is>
       </c>
     </row>
@@ -14978,14 +14978,14 @@
         <v>220000</v>
       </c>
       <c r="B611" t="n">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="C611" t="n">
         <v>3</v>
       </c>
       <c r="D611" t="inlineStr">
         <is>
-          <t>Debrecen, Komlóssy street</t>
+          <t>Debrecen, Simonyi</t>
         </is>
       </c>
       <c r="E611" t="n">
@@ -14993,7 +14993,7 @@
       </c>
       <c r="F611" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/komlossy-street-near-med-uni-beautiful-2-bedroom-living-room-apartment-for-rent/</t>
+          <t>https://www.findahome.hu/ingatlanok/simonyi-street-flat-rent/</t>
         </is>
       </c>
     </row>
@@ -15026,14 +15026,14 @@
         <v>220000</v>
       </c>
       <c r="B613" t="n">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="C613" t="n">
         <v>3</v>
       </c>
       <c r="D613" t="inlineStr">
         <is>
-          <t>Debrecen, Simonyi</t>
+          <t>Debrecen, Serház</t>
         </is>
       </c>
       <c r="E613" t="n">
@@ -15041,7 +15041,7 @@
       </c>
       <c r="F613" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/simonyi-street-flat-rent/</t>
+          <t>https://www.findahome.hu/ingatlanok/debrecen-serhaz-utca-2-bedroom-living-room-flat-for-rent/</t>
         </is>
       </c>
     </row>
@@ -15050,14 +15050,14 @@
         <v>220000</v>
       </c>
       <c r="B614" t="n">
-        <v>65</v>
+        <v>93</v>
       </c>
       <c r="C614" t="n">
         <v>3</v>
       </c>
       <c r="D614" t="inlineStr">
         <is>
-          <t>Debrecen, Arany János</t>
+          <t>Debrecen, Komlóssy street</t>
         </is>
       </c>
       <c r="E614" t="n">
@@ -15065,7 +15065,7 @@
       </c>
       <c r="F614" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/city-center-2-bedroom-american-style-kitchen-apartment-for-rent/</t>
+          <t>https://www.findahome.hu/ingatlanok/komlossy-street-near-med-uni-beautiful-2-bedroom-living-room-apartment-for-rent/</t>
         </is>
       </c>
     </row>
@@ -15074,14 +15074,14 @@
         <v>230000</v>
       </c>
       <c r="B615" t="n">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C615" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D615" t="inlineStr">
         <is>
-          <t>Debrecen, Füredi</t>
+          <t>Debrecen, Dóczy Park</t>
         </is>
       </c>
       <c r="E615" t="n">
@@ -15089,7 +15089,7 @@
       </c>
       <c r="F615" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/apartment-for-rent-in-debrecen-next-to-the-university-of-agriculture/</t>
+          <t>https://www.findahome.hu/ingatlanok/doczy-park-2-bedroom-living-room-flat-for-rent/</t>
         </is>
       </c>
     </row>
@@ -15098,14 +15098,14 @@
         <v>230000</v>
       </c>
       <c r="B616" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C616" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D616" t="inlineStr">
         <is>
-          <t>, Széchenyi street</t>
+          <t>Debrecen, Hadházi út</t>
         </is>
       </c>
       <c r="E616" t="n">
@@ -15113,7 +15113,7 @@
       </c>
       <c r="F616" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/szechenyi-corner-city-center-2-bedroom-living-room-brand-new-flat-for-rent-2/</t>
+          <t>https://debrecenrent.hu/for-rent/flat/debrecen-hadhazi-ut/218454/</t>
         </is>
       </c>
     </row>
@@ -15122,16 +15122,22 @@
         <v>230000</v>
       </c>
       <c r="B617" t="n">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C617" t="n">
-        <v>1</v>
-      </c>
-      <c r="D617" t="inlineStr"/>
-      <c r="E617" t="inlineStr"/>
+        <v>3</v>
+      </c>
+      <c r="D617" t="inlineStr">
+        <is>
+          <t>Debrecen, Károli Gáspár</t>
+        </is>
+      </c>
+      <c r="E617" t="n">
+        <v>1</v>
+      </c>
       <c r="F617" t="inlineStr">
         <is>
-          <t>https://www.greatforest.hu/property/98613-debrecen-jozsa-lower-flat</t>
+          <t>https://www.findahome.hu/ingatlanok/flat-for-rent-karoli-gaspar-street/</t>
         </is>
       </c>
     </row>
@@ -15140,22 +15146,22 @@
         <v>230000</v>
       </c>
       <c r="B618" t="n">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C618" t="n">
         <v>3</v>
       </c>
       <c r="D618" t="inlineStr">
         <is>
-          <t>Debrecen, Dóczy Park</t>
+          <t>Debrecen, Víztorony</t>
         </is>
       </c>
       <c r="E618" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F618" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/doczy-park-2-bedroom-living-room-flat-for-rent/</t>
+          <t>https://www.findahome.hu/ingatlanok/debrecen-3-separate-room-close-to-the-otemeto-kassai-campus/</t>
         </is>
       </c>
     </row>
@@ -15164,14 +15170,14 @@
         <v>230000</v>
       </c>
       <c r="B619" t="n">
-        <v>96</v>
+        <v>61</v>
       </c>
       <c r="C619" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D619" t="inlineStr">
         <is>
-          <t>Debrecen, Tímár street</t>
+          <t>, Széchenyi street</t>
         </is>
       </c>
       <c r="E619" t="n">
@@ -15179,7 +15185,7 @@
       </c>
       <c r="F619" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/timar-street-exclusively-designed-3-bedroom-living-room-flat-available/</t>
+          <t>https://www.findahome.hu/ingatlanok/szechenyi-corner-city-center-2-bedroom-living-room-brand-new-flat-for-rent-2/</t>
         </is>
       </c>
     </row>
@@ -15188,14 +15194,14 @@
         <v>230000</v>
       </c>
       <c r="B620" t="n">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C620" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D620" t="inlineStr">
         <is>
-          <t>Debrecen, Károli Gáspár</t>
+          <t>Debrecen, Füredi</t>
         </is>
       </c>
       <c r="E620" t="n">
@@ -15203,7 +15209,7 @@
       </c>
       <c r="F620" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/flat-for-rent-karoli-gaspar-street/</t>
+          <t>https://www.findahome.hu/ingatlanok/apartment-for-rent-in-debrecen-next-to-the-university-of-agriculture/</t>
         </is>
       </c>
     </row>
@@ -15212,22 +15218,22 @@
         <v>230000</v>
       </c>
       <c r="B621" t="n">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="C621" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D621" t="inlineStr">
         <is>
-          <t>Debrecen, Víztorony</t>
+          <t>Debrecen, Gönczy Pál utca</t>
         </is>
       </c>
       <c r="E621" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F621" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/debrecen-3-separate-room-close-to-the-otemeto-kassai-campus/</t>
+          <t>https://debrecenrent.hu/for-rent/flat/debrecen-gonczy-pal-utca/216064/</t>
         </is>
       </c>
     </row>
@@ -15241,17 +15247,11 @@
       <c r="C622" t="n">
         <v>1</v>
       </c>
-      <c r="D622" t="inlineStr">
-        <is>
-          <t>Debrecen, Gönczy Pál utca</t>
-        </is>
-      </c>
-      <c r="E622" t="n">
-        <v>1</v>
-      </c>
+      <c r="D622" t="inlineStr"/>
+      <c r="E622" t="inlineStr"/>
       <c r="F622" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/flat/debrecen-gonczy-pal-utca/216064/</t>
+          <t>https://www.greatforest.hu/property/98613-debrecen-jozsa-lower-flat</t>
         </is>
       </c>
     </row>
@@ -15260,14 +15260,14 @@
         <v>230000</v>
       </c>
       <c r="B623" t="n">
-        <v>59</v>
+        <v>96</v>
       </c>
       <c r="C623" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D623" t="inlineStr">
         <is>
-          <t>Debrecen, Hadházi út</t>
+          <t>Debrecen, Tímár street</t>
         </is>
       </c>
       <c r="E623" t="n">
@@ -15275,7 +15275,7 @@
       </c>
       <c r="F623" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/flat/debrecen-hadhazi-ut/218454/</t>
+          <t>https://www.findahome.hu/ingatlanok/timar-street-exclusively-designed-3-bedroom-living-room-flat-available/</t>
         </is>
       </c>
     </row>
@@ -15356,22 +15356,22 @@
         <v>240000</v>
       </c>
       <c r="B627" t="n">
-        <v>54</v>
+        <v>90</v>
       </c>
       <c r="C627" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D627" t="inlineStr">
         <is>
-          <t>Debrecen, Nagy Lajos király tér</t>
+          <t>Debrecen, Lilla köz</t>
         </is>
       </c>
       <c r="E627" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F627" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/flat/debrecen-nagy-lajos-kiraly-ter/218134/</t>
+          <t>https://www.findahome.hu/ingatlanok/debrecen-lilla-koz-new-modern-flat-for-rent/</t>
         </is>
       </c>
     </row>
@@ -15380,14 +15380,14 @@
         <v>240000</v>
       </c>
       <c r="B628" t="n">
-        <v>105</v>
+        <v>54</v>
       </c>
       <c r="C628" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D628" t="inlineStr">
         <is>
-          <t>Debrecen, Hatvani István street</t>
+          <t>Debrecen, Nagy Lajos király tér</t>
         </is>
       </c>
       <c r="E628" t="n">
@@ -15395,7 +15395,7 @@
       </c>
       <c r="F628" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/debrecen-hatvani-istvan-street-2-bedroom-living-room-105-sqm-flat-for-rent/</t>
+          <t>https://debrecenrent.hu/for-rent/flat/debrecen-nagy-lajos-kiraly-ter/218134/</t>
         </is>
       </c>
     </row>
@@ -15404,22 +15404,22 @@
         <v>240000</v>
       </c>
       <c r="B629" t="n">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="C629" t="n">
         <v>3</v>
       </c>
       <c r="D629" t="inlineStr">
         <is>
-          <t>Debrecen, Lilla köz</t>
+          <t>Debrecen, Hatvani István street</t>
         </is>
       </c>
       <c r="E629" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F629" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/debrecen-lilla-koz-new-modern-flat-for-rent/</t>
+          <t>https://www.findahome.hu/ingatlanok/debrecen-hatvani-istvan-street-2-bedroom-living-room-105-sqm-flat-for-rent/</t>
         </is>
       </c>
     </row>
@@ -15476,22 +15476,16 @@
         <v>250000</v>
       </c>
       <c r="B632" t="n">
-        <v>65</v>
+        <v>91</v>
       </c>
       <c r="C632" t="n">
         <v>3</v>
       </c>
-      <c r="D632" t="inlineStr">
-        <is>
-          <t>Debrecen, Apafi street</t>
-        </is>
-      </c>
-      <c r="E632" t="n">
-        <v>1</v>
-      </c>
+      <c r="D632" t="inlineStr"/>
+      <c r="E632" t="inlineStr"/>
       <c r="F632" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/debrecen-newer-building-apafi-street-2-bedroom-living-room-terrace-flat-for-rent/</t>
+          <t>https://www.greatforest.hu/property/99332-debrecen-bem-square-office-in-office-building</t>
         </is>
       </c>
     </row>
@@ -15524,16 +15518,22 @@
         <v>250000</v>
       </c>
       <c r="B634" t="n">
-        <v>91</v>
+        <v>65</v>
       </c>
       <c r="C634" t="n">
         <v>3</v>
       </c>
-      <c r="D634" t="inlineStr"/>
-      <c r="E634" t="inlineStr"/>
+      <c r="D634" t="inlineStr">
+        <is>
+          <t>Debrecen, Apafi street</t>
+        </is>
+      </c>
+      <c r="E634" t="n">
+        <v>1</v>
+      </c>
       <c r="F634" t="inlineStr">
         <is>
-          <t>https://www.greatforest.hu/property/99332-debrecen-bem-square-office-in-office-building</t>
+          <t>https://www.findahome.hu/ingatlanok/debrecen-newer-building-apafi-street-2-bedroom-living-room-terrace-flat-for-rent/</t>
         </is>
       </c>
     </row>
@@ -15968,22 +15968,16 @@
         <v>280000</v>
       </c>
       <c r="B653" t="n">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="C653" t="n">
-        <v>2</v>
-      </c>
-      <c r="D653" t="inlineStr">
-        <is>
-          <t>Debrecen, Egyetem tér</t>
-        </is>
-      </c>
-      <c r="E653" t="n">
-        <v>1</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="D653" t="inlineStr"/>
+      <c r="E653" t="inlineStr"/>
       <c r="F653" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/university-residence-new-building-next-to-the-uni-1-bedroom-living-room-flat-for-rent/</t>
+          <t>https://www.greatforest.hu/property/99021-debrecen-city-center-block-of-flats</t>
         </is>
       </c>
     </row>
@@ -15992,16 +15986,16 @@
         <v>280000</v>
       </c>
       <c r="B654" t="n">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C654" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D654" t="inlineStr"/>
       <c r="E654" t="inlineStr"/>
       <c r="F654" t="inlineStr">
         <is>
-          <t>https://www.greatforest.hu/property/99021-debrecen-city-center-block-of-flats</t>
+          <t>https://www.greatforest.hu/property/97856-debrecen-city-center-office-not-in-office-building</t>
         </is>
       </c>
     </row>
@@ -16010,16 +16004,22 @@
         <v>280000</v>
       </c>
       <c r="B655" t="n">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="C655" t="n">
-        <v>3</v>
-      </c>
-      <c r="D655" t="inlineStr"/>
-      <c r="E655" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="D655" t="inlineStr">
+        <is>
+          <t>Debrecen, Egyetem tér</t>
+        </is>
+      </c>
+      <c r="E655" t="n">
+        <v>1</v>
+      </c>
       <c r="F655" t="inlineStr">
         <is>
-          <t>https://www.greatforest.hu/property/97856-debrecen-city-center-office-not-in-office-building</t>
+          <t>https://www.findahome.hu/ingatlanok/university-residence-new-building-next-to-the-uni-1-bedroom-living-room-flat-for-rent/</t>
         </is>
       </c>
     </row>
@@ -16043,43 +16043,49 @@
     </row>
     <row r="657">
       <c r="A657" t="n">
-        <v>290000</v>
+        <v>295000</v>
       </c>
       <c r="B657" t="n">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="C657" t="n">
-        <v>2</v>
-      </c>
-      <c r="D657" t="inlineStr"/>
-      <c r="E657" t="inlineStr"/>
+        <v>4</v>
+      </c>
+      <c r="D657" t="inlineStr">
+        <is>
+          <t>Debrecen, Nagyerdei körút</t>
+        </is>
+      </c>
+      <c r="E657" t="n">
+        <v>2</v>
+      </c>
       <c r="F657" t="inlineStr">
         <is>
-          <t>https://www.greatforest.hu/property/65827-debrecen-close-to-bem-square-part-of-a-house</t>
+          <t>https://www.findahome.hu/ingatlanok/nagyerdei-krt-beautiful-2-levels-home-with-4-rooms-available-for-rent/</t>
         </is>
       </c>
     </row>
     <row r="658">
       <c r="A658" t="n">
-        <v>295000</v>
+        <v>300000</v>
       </c>
       <c r="B658" t="n">
-        <v>143</v>
+        <v>68</v>
       </c>
       <c r="C658" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D658" t="inlineStr">
         <is>
-          <t>Debrecen, Nagyerdei körút</t>
+          <t>Debrecen, Csapó utca</t>
         </is>
       </c>
       <c r="E658" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F658" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/nagyerdei-krt-beautiful-2-levels-home-with-4-rooms-available-for-rent/</t>
+          <t>https://debrecenrent.hu/for-rent/flat/debrecen-csapo-utca/218738/</t>
         </is>
       </c>
     </row>
@@ -16088,22 +16094,16 @@
         <v>300000</v>
       </c>
       <c r="B659" t="n">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="C659" t="n">
         <v>3</v>
       </c>
-      <c r="D659" t="inlineStr">
-        <is>
-          <t>Debrecen, Párizsi udvar</t>
-        </is>
-      </c>
-      <c r="E659" t="n">
-        <v>1</v>
-      </c>
+      <c r="D659" t="inlineStr"/>
+      <c r="E659" t="inlineStr"/>
       <c r="F659" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/debrecen-parizsi-udvar-3-room-70-sqm-flat-for-rent/</t>
+          <t>https://www.greatforest.hu/property/100455-debrecen-flat</t>
         </is>
       </c>
     </row>
@@ -16112,16 +16112,22 @@
         <v>300000</v>
       </c>
       <c r="B660" t="n">
-        <v>67</v>
+        <v>100</v>
       </c>
       <c r="C660" t="n">
-        <v>3</v>
-      </c>
-      <c r="D660" t="inlineStr"/>
-      <c r="E660" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="D660" t="inlineStr">
+        <is>
+          <t>Debrecen, Bem tér</t>
+        </is>
+      </c>
+      <c r="E660" t="n">
+        <v>2</v>
+      </c>
       <c r="F660" t="inlineStr">
         <is>
-          <t>https://www.greatforest.hu/property/101102-debrecen-city-center-flat</t>
+          <t>https://debrecenrent.hu/for-rent/flat/debrecen-bem-ter/163005/</t>
         </is>
       </c>
     </row>
@@ -16130,22 +16136,16 @@
         <v>300000</v>
       </c>
       <c r="B661" t="n">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="C661" t="n">
         <v>2</v>
       </c>
-      <c r="D661" t="inlineStr">
-        <is>
-          <t>Debrecen, Antall József utca</t>
-        </is>
-      </c>
-      <c r="E661" t="n">
-        <v>1</v>
-      </c>
+      <c r="D661" t="inlineStr"/>
+      <c r="E661" t="inlineStr"/>
       <c r="F661" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/flat/debrecen-antall-jozsef-utca/218121/</t>
+          <t>https://www.greatforest.hu/property/69432-debrecen-greatforest-area-flat</t>
         </is>
       </c>
     </row>
@@ -16154,14 +16154,14 @@
         <v>300000</v>
       </c>
       <c r="B662" t="n">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C662" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D662" t="inlineStr">
         <is>
-          <t>Debrecen, Bólyai street</t>
+          <t>Debrecen, Antall József utca</t>
         </is>
       </c>
       <c r="E662" t="n">
@@ -16169,7 +16169,7 @@
       </c>
       <c r="F662" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/bolyai-street-brand-new-beautiful-luxurious-apartment-with-2-bedrooms-for-rent/</t>
+          <t>https://debrecenrent.hu/for-rent/flat/debrecen-antall-jozsef-utca/218121/</t>
         </is>
       </c>
     </row>
@@ -16178,14 +16178,14 @@
         <v>300000</v>
       </c>
       <c r="B663" t="n">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C663" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D663" t="inlineStr">
         <is>
-          <t>Debrecen, Csapó utca</t>
+          <t>Debrecen, Párizsi udvar</t>
         </is>
       </c>
       <c r="E663" t="n">
@@ -16193,7 +16193,7 @@
       </c>
       <c r="F663" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/flat/debrecen-csapo-utca/218738/</t>
+          <t>https://www.findahome.hu/ingatlanok/debrecen-parizsi-udvar-3-room-70-sqm-flat-for-rent/</t>
         </is>
       </c>
     </row>
@@ -16202,22 +16202,16 @@
         <v>300000</v>
       </c>
       <c r="B664" t="n">
-        <v>100</v>
+        <v>67</v>
       </c>
       <c r="C664" t="n">
-        <v>2</v>
-      </c>
-      <c r="D664" t="inlineStr">
-        <is>
-          <t>Debrecen, Bem tér</t>
-        </is>
-      </c>
-      <c r="E664" t="n">
-        <v>2</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="D664" t="inlineStr"/>
+      <c r="E664" t="inlineStr"/>
       <c r="F664" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/flat/debrecen-bem-ter/163005/</t>
+          <t>https://www.greatforest.hu/property/101102-debrecen-city-center-flat</t>
         </is>
       </c>
     </row>
@@ -16226,16 +16220,22 @@
         <v>300000</v>
       </c>
       <c r="B665" t="n">
-        <v>53</v>
+        <v>78</v>
       </c>
       <c r="C665" t="n">
         <v>3</v>
       </c>
-      <c r="D665" t="inlineStr"/>
-      <c r="E665" t="inlineStr"/>
+      <c r="D665" t="inlineStr">
+        <is>
+          <t>Debrecen, Poroszlay</t>
+        </is>
+      </c>
+      <c r="E665" t="n">
+        <v>1</v>
+      </c>
       <c r="F665" t="inlineStr">
         <is>
-          <t>https://www.greatforest.hu/property/100455-debrecen-flat</t>
+          <t>https://www.findahome.hu/ingatlanok/apartment-for-rent-in-debrecen-on-poroszlay-ut/</t>
         </is>
       </c>
     </row>
@@ -16262,32 +16262,38 @@
         <v>300000</v>
       </c>
       <c r="B667" t="n">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="C667" t="n">
-        <v>2</v>
-      </c>
-      <c r="D667" t="inlineStr"/>
-      <c r="E667" t="inlineStr"/>
+        <v>3</v>
+      </c>
+      <c r="D667" t="inlineStr">
+        <is>
+          <t>Debrecen, Bólyai street</t>
+        </is>
+      </c>
+      <c r="E667" t="n">
+        <v>1</v>
+      </c>
       <c r="F667" t="inlineStr">
         <is>
-          <t>https://www.greatforest.hu/property/69432-debrecen-greatforest-area-flat</t>
+          <t>https://www.findahome.hu/ingatlanok/bolyai-street-brand-new-beautiful-luxurious-apartment-with-2-bedrooms-for-rent/</t>
         </is>
       </c>
     </row>
     <row r="668">
       <c r="A668" t="n">
-        <v>300000</v>
+        <v>315000</v>
       </c>
       <c r="B668" t="n">
-        <v>78</v>
+        <v>45</v>
       </c>
       <c r="C668" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D668" t="inlineStr">
         <is>
-          <t>Debrecen, Poroszlay</t>
+          <t>Debrecen, Hatvani István utca</t>
         </is>
       </c>
       <c r="E668" t="n">
@@ -16295,7 +16301,7 @@
       </c>
       <c r="F668" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/apartment-for-rent-in-debrecen-on-poroszlay-ut/</t>
+          <t>https://debrecenrent.hu/for-rent/flat/debrecen-hatvani-istvan-utca/219937/</t>
         </is>
       </c>
     </row>
@@ -16319,7 +16325,7 @@
       </c>
       <c r="F669" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/flat/debrecen-hatvani-istvan-utca/219994/</t>
+          <t>https://debrecenrent.hu/for-rent/flat/debrecen-hatvani-istvan-utca/219974/</t>
         </is>
       </c>
     </row>
@@ -16343,7 +16349,7 @@
       </c>
       <c r="F670" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/flat/debrecen-hatvani-istvan-utca/219937/</t>
+          <t>https://debrecenrent.hu/for-rent/flat/debrecen-hatvani-istvan-utca/219994/</t>
         </is>
       </c>
     </row>
@@ -16367,7 +16373,7 @@
       </c>
       <c r="F671" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/flat/debrecen-hatvani-istvan-utca/220005/</t>
+          <t>https://debrecenrent.hu/for-rent/flat/debrecen-hatvani-istvan-utca/219906/</t>
         </is>
       </c>
     </row>
@@ -16391,7 +16397,7 @@
       </c>
       <c r="F672" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/flat/debrecen-hatvani-istvan-utca/219959/</t>
+          <t>https://debrecenrent.hu/for-rent/flat/debrecen-hatvani-istvan-utca/220005/</t>
         </is>
       </c>
     </row>
@@ -16439,31 +16445,25 @@
       </c>
       <c r="F674" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/flat/debrecen-hatvani-istvan-utca/219974/</t>
+          <t>https://debrecenrent.hu/for-rent/flat/debrecen-hatvani-istvan-utca/219959/</t>
         </is>
       </c>
     </row>
     <row r="675">
       <c r="A675" t="n">
-        <v>315000</v>
+        <v>320000</v>
       </c>
       <c r="B675" t="n">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C675" t="n">
         <v>1</v>
       </c>
-      <c r="D675" t="inlineStr">
-        <is>
-          <t>Debrecen, Hatvani István utca</t>
-        </is>
-      </c>
-      <c r="E675" t="n">
-        <v>1</v>
-      </c>
+      <c r="D675" t="inlineStr"/>
+      <c r="E675" t="inlineStr"/>
       <c r="F675" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/flat/debrecen-hatvani-istvan-utca/219906/</t>
+          <t>https://www.greatforest.hu/property/99511-debrecen-close-to-main-campus-flat</t>
         </is>
       </c>
     </row>
@@ -16472,16 +16472,22 @@
         <v>320000</v>
       </c>
       <c r="B676" t="n">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="C676" t="n">
-        <v>1</v>
-      </c>
-      <c r="D676" t="inlineStr"/>
-      <c r="E676" t="inlineStr"/>
+        <v>3</v>
+      </c>
+      <c r="D676" t="inlineStr">
+        <is>
+          <t>Debrecen, Széchenyi utca</t>
+        </is>
+      </c>
+      <c r="E676" t="n">
+        <v>1</v>
+      </c>
       <c r="F676" t="inlineStr">
         <is>
-          <t>https://www.greatforest.hu/property/99511-debrecen-close-to-main-campus-flat</t>
+          <t>https://debrecenrent.hu/for-rent/flat/debrecen-szechenyi-utca/219826/</t>
         </is>
       </c>
     </row>
@@ -16490,56 +16496,56 @@
         <v>320000</v>
       </c>
       <c r="B677" t="n">
-        <v>89</v>
+        <v>42</v>
       </c>
       <c r="C677" t="n">
-        <v>3</v>
-      </c>
-      <c r="D677" t="inlineStr">
-        <is>
-          <t>Debrecen, Széchenyi utca</t>
-        </is>
-      </c>
-      <c r="E677" t="n">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D677" t="inlineStr"/>
+      <c r="E677" t="inlineStr"/>
       <c r="F677" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/flat/debrecen-szechenyi-utca/219826/</t>
+          <t>https://www.greatforest.hu/property/99510-debrecen-close-to-main-campus-flat</t>
         </is>
       </c>
     </row>
     <row r="678">
       <c r="A678" t="n">
-        <v>320000</v>
+        <v>330000</v>
       </c>
       <c r="B678" t="n">
-        <v>42</v>
+        <v>80</v>
       </c>
       <c r="C678" t="n">
-        <v>1</v>
-      </c>
-      <c r="D678" t="inlineStr"/>
-      <c r="E678" t="inlineStr"/>
+        <v>3</v>
+      </c>
+      <c r="D678" t="inlineStr">
+        <is>
+          <t>Debrecen, Hatvan</t>
+        </is>
+      </c>
+      <c r="E678" t="n">
+        <v>1</v>
+      </c>
       <c r="F678" t="inlineStr">
         <is>
-          <t>https://www.greatforest.hu/property/99510-debrecen-close-to-main-campus-flat</t>
+          <t>https://www.findahome.hu/ingatlanok/apartment-for-rent-on-hatvan-street/</t>
         </is>
       </c>
     </row>
     <row r="679">
       <c r="A679" t="n">
-        <v>330000</v>
+        <v>350000</v>
       </c>
       <c r="B679" t="n">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="C679" t="n">
         <v>3</v>
       </c>
       <c r="D679" t="inlineStr">
         <is>
-          <t>Debrecen, Hatvan</t>
+          <t>Debrecen, Menyhárt József tér</t>
         </is>
       </c>
       <c r="E679" t="n">
@@ -16547,7 +16553,7 @@
       </c>
       <c r="F679" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/apartment-for-rent-on-hatvan-street/</t>
+          <t>https://www.findahome.hu/ingatlanok/luxury-apartment-for-rent-in-menyhart-jozsef-ter/</t>
         </is>
       </c>
     </row>
@@ -16556,22 +16562,22 @@
         <v>350000</v>
       </c>
       <c r="B680" t="n">
-        <v>65</v>
+        <v>130</v>
       </c>
       <c r="C680" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D680" t="inlineStr">
         <is>
-          <t>Debrecen, Menyhárt József tér</t>
+          <t>Debrecen, Akadémia utca</t>
         </is>
       </c>
       <c r="E680" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F680" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/luxury-apartment-for-rent-in-menyhart-jozsef-ter/</t>
+          <t>https://debrecenrent.hu/for-rent/house/debrecen-akademia-utca/217736/</t>
         </is>
       </c>
     </row>
@@ -16580,22 +16586,16 @@
         <v>350000</v>
       </c>
       <c r="B681" t="n">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="C681" t="n">
         <v>4</v>
       </c>
-      <c r="D681" t="inlineStr">
-        <is>
-          <t>Debrecen, Akadémia utca</t>
-        </is>
-      </c>
-      <c r="E681" t="n">
-        <v>2</v>
-      </c>
+      <c r="D681" t="inlineStr"/>
+      <c r="E681" t="inlineStr"/>
       <c r="F681" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/house/debrecen-akademia-utca/217736/</t>
+          <t>https://www.greatforest.hu/property/89979-debrecen-city-center-office-not-in-office-building</t>
         </is>
       </c>
     </row>
@@ -16604,74 +16604,80 @@
         <v>350000</v>
       </c>
       <c r="B682" t="n">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C682" t="n">
         <v>4</v>
       </c>
-      <c r="D682" t="inlineStr"/>
-      <c r="E682" t="inlineStr"/>
+      <c r="D682" t="inlineStr">
+        <is>
+          <t>Debrecen, Bem tér</t>
+        </is>
+      </c>
+      <c r="E682" t="n">
+        <v>2</v>
+      </c>
       <c r="F682" t="inlineStr">
         <is>
-          <t>https://www.greatforest.hu/property/89979-debrecen-city-center-office-not-in-office-building</t>
+          <t>https://www.findahome.hu/ingatlanok/bem-ter-3-bedroom-living-room-with-dining-area-2-bathroom/</t>
         </is>
       </c>
     </row>
     <row r="683">
       <c r="A683" t="n">
-        <v>350000</v>
+        <v>375000</v>
       </c>
       <c r="B683" t="n">
-        <v>112</v>
+        <v>82</v>
       </c>
       <c r="C683" t="n">
         <v>4</v>
       </c>
-      <c r="D683" t="inlineStr">
-        <is>
-          <t>Debrecen, Bem tér</t>
-        </is>
-      </c>
-      <c r="E683" t="n">
-        <v>2</v>
-      </c>
+      <c r="D683" t="inlineStr"/>
+      <c r="E683" t="inlineStr"/>
       <c r="F683" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/bem-ter-3-bedroom-living-room-with-dining-area-2-bathroom/</t>
+          <t>https://www.greatforest.hu/property/96519-debrecen-greatforest-area-flat</t>
         </is>
       </c>
     </row>
     <row r="684">
       <c r="A684" t="n">
-        <v>375000</v>
+        <v>380000</v>
       </c>
       <c r="B684" t="n">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="C684" t="n">
         <v>4</v>
       </c>
-      <c r="D684" t="inlineStr"/>
-      <c r="E684" t="inlineStr"/>
+      <c r="D684" t="inlineStr">
+        <is>
+          <t>Debrecen, -</t>
+        </is>
+      </c>
+      <c r="E684" t="n">
+        <v>1</v>
+      </c>
       <c r="F684" t="inlineStr">
         <is>
-          <t>https://www.greatforest.hu/property/96519-debrecen-greatforest-area-flat</t>
+          <t>https://www.findahome.hu/ingatlanok/debrecen-house-for-rent-with-3-bedrooms-living-room/</t>
         </is>
       </c>
     </row>
     <row r="685">
       <c r="A685" t="n">
-        <v>380000</v>
+        <v>385000</v>
       </c>
       <c r="B685" t="n">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="C685" t="n">
         <v>4</v>
       </c>
       <c r="D685" t="inlineStr">
         <is>
-          <t>Debrecen, -</t>
+          <t>Debrecen, Vas Gereben</t>
         </is>
       </c>
       <c r="E685" t="n">
@@ -16679,23 +16685,23 @@
       </c>
       <c r="F685" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/debrecen-house-for-rent-with-3-bedrooms-living-room/</t>
+          <t>https://www.findahome.hu/ingatlanok/17339/</t>
         </is>
       </c>
     </row>
     <row r="686">
       <c r="A686" t="n">
-        <v>385000</v>
+        <v>390000</v>
       </c>
       <c r="B686" t="n">
-        <v>90</v>
+        <v>115</v>
       </c>
       <c r="C686" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D686" t="inlineStr">
         <is>
-          <t>Debrecen, Vas Gereben</t>
+          <t>Debrecen, Csapó utca</t>
         </is>
       </c>
       <c r="E686" t="n">
@@ -16703,7 +16709,7 @@
       </c>
       <c r="F686" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/17339/</t>
+          <t>https://debrecenrent.hu/for-rent/flat/debrecen-csapo-utca/219320/</t>
         </is>
       </c>
     </row>
@@ -16712,14 +16718,14 @@
         <v>390000</v>
       </c>
       <c r="B687" t="n">
-        <v>115</v>
+        <v>75</v>
       </c>
       <c r="C687" t="n">
         <v>3</v>
       </c>
       <c r="D687" t="inlineStr">
         <is>
-          <t>Debrecen, Csapó utca</t>
+          <t>Debrecen, Nagyerdei körút</t>
         </is>
       </c>
       <c r="E687" t="n">
@@ -16727,23 +16733,23 @@
       </c>
       <c r="F687" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/flat/debrecen-csapo-utca/219320/</t>
+          <t>https://debrecenrent.hu/for-rent/flat/debrecen-nagyerdei-korut/213647/</t>
         </is>
       </c>
     </row>
     <row r="688">
       <c r="A688" t="n">
-        <v>390000</v>
+        <v>395000</v>
       </c>
       <c r="B688" t="n">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C688" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D688" t="inlineStr">
         <is>
-          <t>Debrecen, Nagyerdei körút</t>
+          <t>Debrecen, Garai utca</t>
         </is>
       </c>
       <c r="E688" t="n">
@@ -16751,7 +16757,7 @@
       </c>
       <c r="F688" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/flat/debrecen-nagyerdei-korut/213647/</t>
+          <t>https://debrecenrent.hu/for-rent/flat/debrecen-garai-utca/217183/</t>
         </is>
       </c>
     </row>
@@ -16760,7 +16766,7 @@
         <v>395000</v>
       </c>
       <c r="B689" t="n">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="C689" t="n">
         <v>2</v>
@@ -16771,51 +16777,51 @@
         </is>
       </c>
       <c r="E689" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F689" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/flat/debrecen-garai-utca/217183/</t>
+          <t>https://debrecenrent.hu/for-rent/flat/debrecen-garai-utca/217196/</t>
         </is>
       </c>
     </row>
     <row r="690">
       <c r="A690" t="n">
-        <v>395000</v>
+        <v>410000</v>
       </c>
       <c r="B690" t="n">
-        <v>83</v>
+        <v>106</v>
       </c>
       <c r="C690" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D690" t="inlineStr">
         <is>
-          <t>Debrecen, Garai utca</t>
+          <t>Debrecen, Piac</t>
         </is>
       </c>
       <c r="E690" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F690" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/flat/debrecen-garai-utca/217196/</t>
+          <t>https://www.findahome.hu/ingatlanok/debrecen-city-center-piac-street-2-bedroom-living-room-flat-for-rent/</t>
         </is>
       </c>
     </row>
     <row r="691">
       <c r="A691" t="n">
-        <v>410000</v>
+        <v>420000</v>
       </c>
       <c r="B691" t="n">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="C691" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D691" t="inlineStr">
         <is>
-          <t>Debrecen, Piac</t>
+          <t>Debrecen, Rákóczi</t>
         </is>
       </c>
       <c r="E691" t="n">
@@ -16823,31 +16829,25 @@
       </c>
       <c r="F691" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/debrecen-city-center-piac-street-2-bedroom-living-room-flat-for-rent/</t>
+          <t>https://www.findahome.hu/ingatlanok/debrecen-belvaros-3-bedroom-living-room-unfurnished-apartament-for-rent/</t>
         </is>
       </c>
     </row>
     <row r="692">
       <c r="A692" t="n">
-        <v>420000</v>
+        <v>480000</v>
       </c>
       <c r="B692" t="n">
-        <v>112</v>
+        <v>83</v>
       </c>
       <c r="C692" t="n">
-        <v>4</v>
-      </c>
-      <c r="D692" t="inlineStr">
-        <is>
-          <t>Debrecen, Rákóczi</t>
-        </is>
-      </c>
-      <c r="E692" t="n">
-        <v>1</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="D692" t="inlineStr"/>
+      <c r="E692" t="inlineStr"/>
       <c r="F692" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/debrecen-belvaros-3-bedroom-living-room-unfurnished-apartament-for-rent/</t>
+          <t>https://www.greatforest.hu/property/97187-debrecen-flat</t>
         </is>
       </c>
     </row>
@@ -16856,7 +16856,7 @@
         <v>480000</v>
       </c>
       <c r="B693" t="n">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="C693" t="n">
         <v>3</v>
@@ -16865,49 +16865,55 @@
       <c r="E693" t="inlineStr"/>
       <c r="F693" t="inlineStr">
         <is>
-          <t>https://www.greatforest.hu/property/97187-debrecen-flat</t>
+          <t>https://www.greatforest.hu/property/97186-debrecen-city-center-flat</t>
         </is>
       </c>
     </row>
     <row r="694">
       <c r="A694" t="n">
-        <v>480000</v>
+        <v>490000</v>
       </c>
       <c r="B694" t="n">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="C694" t="n">
-        <v>3</v>
-      </c>
-      <c r="D694" t="inlineStr"/>
-      <c r="E694" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="D694" t="inlineStr">
+        <is>
+          <t>Debrecen, Mikszáth Kálmán utca</t>
+        </is>
+      </c>
+      <c r="E694" t="n">
+        <v>1</v>
+      </c>
       <c r="F694" t="inlineStr">
         <is>
-          <t>https://www.greatforest.hu/property/97186-debrecen-city-center-flat</t>
+          <t>https://debrecenrent.hu/for-rent/flat/debrecen-mikszath-kalman-utca/216981/</t>
         </is>
       </c>
     </row>
     <row r="695">
       <c r="A695" t="n">
-        <v>490000</v>
+        <v>500000</v>
       </c>
       <c r="B695" t="n">
-        <v>52</v>
+        <v>147</v>
       </c>
       <c r="C695" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D695" t="inlineStr">
         <is>
-          <t>Debrecen, Mikszáth Kálmán utca</t>
+          <t>Hajdúszoboszló, Hőforrás utca</t>
         </is>
       </c>
       <c r="E695" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F695" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/flat/debrecen-mikszath-kalman-utca/216981/</t>
+          <t>https://debrecenrent.hu/for-rent/house/hajduszoboszlo-hoforras-utca/214766/</t>
         </is>
       </c>
     </row>
@@ -16916,31 +16922,25 @@
         <v>500000</v>
       </c>
       <c r="B696" t="n">
-        <v>147</v>
+        <v>116</v>
       </c>
       <c r="C696" t="n">
-        <v>3</v>
-      </c>
-      <c r="D696" t="inlineStr">
-        <is>
-          <t>Hajdúszoboszló, Hőforrás utca</t>
-        </is>
-      </c>
-      <c r="E696" t="n">
-        <v>2</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="D696" t="inlineStr"/>
+      <c r="E696" t="inlineStr"/>
       <c r="F696" t="inlineStr">
         <is>
-          <t>https://debrecenrent.hu/for-rent/house/hajduszoboszlo-hoforras-utca/214766/</t>
+          <t>https://www.greatforest.hu/property/101101-debrecen-city-center-flat</t>
         </is>
       </c>
     </row>
     <row r="697">
       <c r="A697" t="n">
-        <v>500000</v>
+        <v>580000</v>
       </c>
       <c r="B697" t="n">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="C697" t="n">
         <v>4</v>
@@ -16949,25 +16949,25 @@
       <c r="E697" t="inlineStr"/>
       <c r="F697" t="inlineStr">
         <is>
-          <t>https://www.greatforest.hu/property/101101-debrecen-city-center-flat</t>
+          <t>https://www.greatforest.hu/property/98425-debrecen-city-center-flat</t>
         </is>
       </c>
     </row>
     <row r="698">
       <c r="A698" t="n">
-        <v>580000</v>
+        <v>595000</v>
       </c>
       <c r="B698" t="n">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C698" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D698" t="inlineStr"/>
       <c r="E698" t="inlineStr"/>
       <c r="F698" t="inlineStr">
         <is>
-          <t>https://www.greatforest.hu/property/98425-debrecen-city-center-flat</t>
+          <t>https://www.greatforest.hu/property/36059-debrecen-kassai-campus-area-flat</t>
         </is>
       </c>
     </row>
@@ -16976,34 +16976,40 @@
         <v>595000</v>
       </c>
       <c r="B699" t="n">
-        <v>92</v>
+        <v>147</v>
       </c>
       <c r="C699" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D699" t="inlineStr"/>
       <c r="E699" t="inlineStr"/>
       <c r="F699" t="inlineStr">
         <is>
-          <t>https://www.greatforest.hu/property/36059-debrecen-kassai-campus-area-flat</t>
+          <t>https://www.greatforest.hu/property/101274-hajduszoboszlo-attached-house</t>
         </is>
       </c>
     </row>
     <row r="700">
       <c r="A700" t="n">
-        <v>595000</v>
+        <v>600000</v>
       </c>
       <c r="B700" t="n">
-        <v>147</v>
+        <v>93</v>
       </c>
       <c r="C700" t="n">
         <v>4</v>
       </c>
-      <c r="D700" t="inlineStr"/>
-      <c r="E700" t="inlineStr"/>
+      <c r="D700" t="inlineStr">
+        <is>
+          <t>Debrecen, Bajcsy-Zsilinszky</t>
+        </is>
+      </c>
+      <c r="E700" t="n">
+        <v>1</v>
+      </c>
       <c r="F700" t="inlineStr">
         <is>
-          <t>https://www.greatforest.hu/property/101274-hajduszoboszlo-attached-house</t>
+          <t>https://www.findahome.hu/ingatlanok/luxury-apartment-for-rent/</t>
         </is>
       </c>
     </row>
@@ -17012,14 +17018,14 @@
         <v>600000</v>
       </c>
       <c r="B701" t="n">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C701" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D701" t="inlineStr">
         <is>
-          <t>Debrecen, Bajcsy-Zsilinszky</t>
+          <t>Debrecen, Hadházi út</t>
         </is>
       </c>
       <c r="E701" t="n">
@@ -17027,53 +17033,29 @@
       </c>
       <c r="F701" t="inlineStr">
         <is>
-          <t>https://www.findahome.hu/ingatlanok/luxury-apartment-for-rent/</t>
+          <t>https://debrecenrent.hu/for-rent/flat/debrecen-hadhazi-ut/219319/</t>
         </is>
       </c>
     </row>
     <row r="702">
       <c r="A702" t="n">
-        <v>600000</v>
+        <v>760000</v>
       </c>
       <c r="B702" t="n">
-        <v>92</v>
+        <v>135</v>
       </c>
       <c r="C702" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D702" t="inlineStr">
         <is>
-          <t>Debrecen, Hadházi út</t>
+          <t>Debrecen, Pacsirta</t>
         </is>
       </c>
       <c r="E702" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F702" t="inlineStr">
-        <is>
-          <t>https://debrecenrent.hu/for-rent/flat/debrecen-hadhazi-ut/219319/</t>
-        </is>
-      </c>
-    </row>
-    <row r="703">
-      <c r="A703" t="n">
-        <v>760000</v>
-      </c>
-      <c r="B703" t="n">
-        <v>135</v>
-      </c>
-      <c r="C703" t="n">
-        <v>4</v>
-      </c>
-      <c r="D703" t="inlineStr">
-        <is>
-          <t>Debrecen, Pacsirta</t>
-        </is>
-      </c>
-      <c r="E703" t="n">
-        <v>0</v>
-      </c>
-      <c r="F703" t="inlineStr">
         <is>
           <t>https://www.findahome.hu/ingatlanok/luxury-house-for-rent-3-bedroom-living-room/</t>
         </is>

</xml_diff>